<commit_message>
2nd Update a SignalMatrix for R2 HkmcFcaAdap
</commit_message>
<xml_diff>
--- a/R2/02_SignalMatrix/HkmcFcaAdap/HkmcFcaAdap_SignalMatrix_V1.xlsx
+++ b/R2/02_SignalMatrix/HkmcFcaAdap/HkmcFcaAdap_SignalMatrix_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HKMC\Features\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soo-jin.ahn\Veoneer\KHT HKMC BN7 FCA Project - SOS and MVS4\01_Engineering\03_SW and FD\ApplicationSoftware\FeatureSignalMatrixs\HkmcFcaAdap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{345847E7-D56C-41D3-9BD6-A37BFB0E82E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F895C6BF-1CD6-41A7-8449-5B293917FBEF}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{345847E7-D56C-41D3-9BD6-A37BFB0E82E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B10CF31-E1AB-48F8-ABB8-75381FF14C64}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="22" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="125">
   <si>
     <t>Change Log</t>
   </si>
@@ -148,56 +148,150 @@
     <t>HFA_OUTPUTS</t>
   </si>
   <si>
-    <t xml:space="preserve">FcaAdap_WrngLvlSta </t>
-  </si>
-  <si>
     <t>enum</t>
   </si>
   <si>
     <t>Output</t>
   </si>
   <si>
-    <t>Cx0 _No_warning
-Cx1 _Warning_Level
-Cx2 _Warning_Level
-Cx3_Warning_Level</t>
-  </si>
-  <si>
-    <t>FcaAdap_WrngSndSta</t>
-  </si>
-  <si>
-    <t>Cx0 _No_warning
-Cx1 _Warning_Level
-Cx2 _Warning_Level
-Cx3 _Warning_Level</t>
-  </si>
-  <si>
-    <t>FcaAdap_PrefillActvReq</t>
-  </si>
-  <si>
-    <t>Cx0_No Pre-fill
-Cx1_Pre-fill act
+    <t>uint8</t>
+  </si>
+  <si>
+    <t>[0..2.55] ,0.01</t>
+  </si>
+  <si>
+    <t>u16</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>[0…255]</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>Cx0_Unknown
+Cx1_Car
+Cx2_Motorcycle
+Cx3_Truck
+Cx4_Pedestrian
+Cx5_Bicycle
+Cx6_GeneralObject</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationBrakeRequest</t>
+  </si>
+  <si>
+    <t>CollisionMitigationBrakeRequest</t>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem</t>
+  </si>
+  <si>
+    <t>Cx0_NoMessage
+Cx1_InterventionLongitudinal
+Cx2_InterventionLateral
+Cx3_InterventionLongitudinalAndInterventionLateral
+Cx4_BrakePulse
+Cx5_CriteriaBrakeMessage</t>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput</t>
+  </si>
+  <si>
+    <t>EgoMotionOutput</t>
+  </si>
+  <si>
+    <t>U32</t>
+  </si>
+  <si>
+    <t>Cx0_Unknown_x000D_
+Cx1_SuccessfulVerification_x000D_
+Cx2_VerificationFailed</t>
+  </si>
+  <si>
+    <t>Cx0_Unknown
+Cx1_SuccessfulVerification
+Cx2_VerificationFailed</t>
+  </si>
+  <si>
+    <t>HVIA_CLU</t>
+  </si>
+  <si>
+    <t>HkmcVehicleInput SWC / FcaAdap SWC</t>
+  </si>
+  <si>
+    <t>HkmcFcaAdap SWC</t>
+  </si>
+  <si>
+    <t>Port Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CollisionMitigationSystem</t>
+  </si>
+  <si>
+    <t>HVIA_OUTPUTS</t>
+  </si>
+  <si>
+    <t>VIPCDDSWC</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInputAdap</t>
+  </si>
+  <si>
+    <t>HkmcVehicleOutPutAdap</t>
+  </si>
+  <si>
+    <t>Cx0_kmperh
+Cx1_MPH
+Cx2_Not_used
+Cx3_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_NoActivation
+Cx1_ActivationLow
+Cx2_ActivationHigh
+Cx3_NotInUse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-25.5…25.6] , 0.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_No_warning
+Cx1_Warning_Level_1
+Cx2_Warning_Level_2
+Cx3_Warning_Level_3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_No_Pre_fill
+Cx1_Pre_fill_act
 Cx2_Reserved
-Cx3_Error Indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FcaAdap_DclReqVal </t>
-  </si>
-  <si>
-    <t>uint8</t>
-  </si>
-  <si>
-    <t>[0..2.55] ,0.01</t>
-  </si>
-  <si>
-    <t>FcaAdap_FullActvReq</t>
+Cx3_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_No_Full_act
-Cx1 _Full_act</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FcaAdap_StbltActvReq </t>
+Cx1_Full_act
+Cx2_Reserved
+Cx3_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_Release_no_alert
@@ -206,20 +300,16 @@
 Cx3_Reserved
 Cx4_Reserved
 Cx5_Reserved
-0x6  Reserved
-0x7 - Reserved</t>
-  </si>
-  <si>
-    <t>FcaAdap_VehStpReq</t>
+Cx6_Reserved
+Cx7_Reserved</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_No_Request
 Cx1_Stop_control_is_required
 Cx2_Reserved
 Cx3_Error_Indicator</t>
-  </si>
-  <si>
-    <t>FcaAdap_OnOffEquipSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_Default
@@ -230,9 +320,7 @@
 Cx5_Reserved
 Cx6_Reserved
 Cx7_Invalid</t>
-  </si>
-  <si>
-    <t>FcaAdap_SysFlrSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_Normal
@@ -243,36 +331,15 @@
 Cx5_Reserved
 Cx6_Reserved
 Cx7_Reserved</t>
-  </si>
-  <si>
-    <t>FcaAdap_RelVel</t>
-  </si>
-  <si>
-    <t>u16</t>
-  </si>
-  <si>
-    <t>[-25.5…25.6] , 0.1</t>
-  </si>
-  <si>
-    <t>FcaAdap_TimetoCllsn</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>[0…255]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>FcaAdap_SnstvtyModRetVal</t>
-  </si>
-  <si>
-    <t>FcaAdap_LongitudinalVelocity</t>
-  </si>
-  <si>
-    <t>S16</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>FcaAdap_ObjectType</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_Unknown
@@ -282,231 +349,336 @@
 Cx4_Pedestrian
 Cx5_Bicycle
 Cx6_GeneralObject</t>
-  </si>
-  <si>
-    <t>FcaAdap_WarningRequest</t>
-  </si>
-  <si>
-    <t>boolean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>FcaAdap_CollisionThreatLevel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_Unknown
 Cx1_ThreatLow
 Cx2_ThreatMedium
 Cx3_ThreatHigh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FcaAdap_DecelerationRequest </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_WrngLvlSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_WrngSndSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_PrefillActvReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_FullActvReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_StbltActvReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_VehStpReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_OnOffEquipSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_SysFlrSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EgoMotionOutput</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_DclReqVal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_RelVel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_TimetoCllsn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_LongitudinalVelocity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_WarningRequest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_DecelerationRequest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>FcaAdap_StandStillRequest</t>
-  </si>
-  <si>
-    <t>bool</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HVIA_CLU</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInput_SpdUnitTyp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInput_Fca1stWrngSetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_Default
+Cx1_LDW_Mode
+Cx2_LKA_Mode
+Cx3_Reserved
+Cx4_Reserved
+Cx5_Reserved
+Cx6_Reserved
+Cx7_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInput_AdasFCASetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>U8(Arxml : F32)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForwardWarningControl</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>U16(Arxml : F32)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arxml : not enum
+(F32)As_Coord2F32.x
+(F32)As_Coord2F32.y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arxml don't have this siganl</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ASP_CollisionMitigationBrakeRequest</t>
-  </si>
-  <si>
-    <t>CollisionMitigationBrakeRequest</t>
-  </si>
-  <si>
-    <t>CollisionMitigationBrakeRequest.DecelerationEnabled</t>
-  </si>
-  <si>
-    <t>CollisionMitigationBrakeRequest.DecelerationRequest</t>
-  </si>
-  <si>
-    <t>CollisionMitigationBrakeRequest.StandStillRequest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ASP_CollisionMitigationSystem</t>
-  </si>
-  <si>
-    <t>ForwardWarningControl</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ForwardWarningControl.WarningRequest</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ForwardWarningControl.ObjectType</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ForwardWarningControl.BrakeGainEnabled</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ForwardWarningControl.BrakeGainRequest</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ForwardWarningControl.BrakeGainMaxDeceleration</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ForwardWarningControl.TimeToCollision</t>
-  </si>
-  <si>
-    <t>U16</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ForwardWarningControl.ObjectId</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ForwardWarningControl.ObjectPosition</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ThreatInformation</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ThreatInformation.BeltActivationLevel</t>
-  </si>
-  <si>
-    <t>Cx0_NoActivation_x000D_
-Cx1_ActivationLow_x000D_
-Cx2_ActivationHigh_x000D_
-Cx3_NotInUse</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ThreatInformation.CollisionThreatLevel</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ThreatInformation.DisplayPostEventMessage</t>
-  </si>
-  <si>
-    <t>Cx0_NoMessage
-Cx1_InterventionLongitudinal
-Cx2_InterventionLateral
-Cx3_InterventionLongitudinalAndInterventionLateral
-Cx4_BrakePulse
-Cx5_CriteriaBrakeMessage</t>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem.ThreatInformation.TimeToBrake</t>
-  </si>
-  <si>
-    <t>ASP_EgoMotionOutput</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.LongitudinalVelocity</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.LongitudinalAcceleration</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.LateralVelocity</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.LateralAcceleration</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.YawRate</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.IsAvailable</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.Timestamp</t>
-  </si>
-  <si>
-    <t>U32</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.LongitudinalVelocityStatus</t>
-  </si>
-  <si>
-    <t>Cx0_Unknown_x000D_
-Cx1_SuccessfulVerification_x000D_
-Cx2_VerificationFailed</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.AccelerationStatus</t>
-  </si>
-  <si>
-    <t>Cx0_Unknown
-Cx1_SuccessfulVerification
-Cx2_VerificationFailed</t>
-  </si>
-  <si>
-    <t>EgoMotionOutput.YawRateStatus</t>
-  </si>
-  <si>
-    <t>HVIA_CLU</t>
-  </si>
-  <si>
-    <t>HkmcVehicleInput_SpdUnitTyp</t>
-  </si>
-  <si>
-    <t>Cx0_kmperh
-Cx1_MPH
-Cx2_Not_used
-Cx3_Error_Indicator</t>
-  </si>
-  <si>
-    <t>HkmcVehicleInput_Fca1stWrngSetReq</t>
-  </si>
-  <si>
-    <t>Cx0_Default_x000D_
-Cx1_LDW_Mode_x000D_
-Cx2_LKA_Mode_x000D_
-Cx3_Reserved_x000D_
-Cx4_Reserved_x000D_
-Cx5_Reserved_x000D_
-Cx6_Reserved_x000D_
-Cx7_Invalid</t>
-  </si>
-  <si>
-    <t>HkmcVehicleInput_AdasFCASetReq </t>
-  </si>
-  <si>
-    <t>HkmcVehicleInput SWC / FcaAdap SWC</t>
-  </si>
-  <si>
-    <t>HkmcFcaAdap SWC</t>
-  </si>
-  <si>
-    <t>Port Type</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CollisionMitigationSystem</t>
-  </si>
-  <si>
-    <t>HVIA_OUTPUTS</t>
-  </si>
-  <si>
-    <t>VIPCDDSWC</t>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>HkmcVehicleInputAdap</t>
-  </si>
-  <si>
-    <t>HkmcVehicleOutPutAdap</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ASP_CollisionMitigationBrakeRequest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.DecelerationEnabled</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ASP_CollisionMitigationBrakeRequest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.DecelerationRequest</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ASP_CollisionMitigationBrakeRequest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.StandStillRequest</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ForwardWarningControl.WarningRequest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ForwardWarningControl.ObjectType</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ForwardWarningControl.BrakeGainEnabled</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ForwardWarningControl.BrakeGainRequest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ForwardWarningControl.BrakeGainMaxDeceleration</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ForwardWarningControl.TimeToCollision</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ForwardWarningControl.ObjectId</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ForwardWarningControl.ObjectPosition</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ThreatInformation.BeltActivationLevel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ThreatInformation.CollisionThreatLevel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ThreatInformation.DisplayPostEventMessage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_CollisionMitigationSystem.ThreatInformation.TimeToBrake</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.LongitudinalVelocity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.LongitudinalAcceleration</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.LateralVelocity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.LateralAcceleration</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.YawRate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.IsAvailable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.Timestamp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.LongitudinalVelocityStatus</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.AccelerationStatus</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_EgoMotionOutput.YawRateStatus</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HFA_OUTPUTS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -517,7 +689,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -526,7 +698,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -534,20 +706,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -555,7 +727,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -563,7 +735,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -571,21 +743,21 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -595,8 +767,32 @@
       <name val="Lucida Sans Unicode"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -686,6 +882,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -1044,7 +1246,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1172,12 +1374,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="15" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="15" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
@@ -1186,7 +1382,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="15" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1204,16 +1399,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1239,6 +1430,44 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="21" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="15" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Good" xfId="13" builtinId="26"/>
@@ -1690,16 +1919,16 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="72.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
+    <col min="4" max="4" width="23.25" customWidth="1"/>
+    <col min="5" max="5" width="72.75" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15" customHeight="1">
+    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1732,7 +1961,7 @@
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
     </row>
-    <row r="2" spans="1:31" ht="15" thickBot="1">
+    <row r="2" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1765,15 +1994,15 @@
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="72"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="67"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1800,7 +2029,7 @@
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
     </row>
-    <row r="4" spans="1:31" ht="15" thickBot="1">
+    <row r="4" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="8" t="s">
         <v>1</v>
@@ -1841,7 +2070,7 @@
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
     </row>
-    <row r="5" spans="1:31" ht="15" thickTop="1">
+    <row r="5" spans="1:31" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="11">
         <v>1</v>
@@ -1884,7 +2113,7 @@
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="16"/>
       <c r="C6" s="27"/>
@@ -1917,7 +2146,7 @@
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -1950,7 +2179,7 @@
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="16"/>
       <c r="C8" s="17"/>
@@ -1983,7 +2212,7 @@
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="11"/>
       <c r="C9" s="13"/>
@@ -2016,7 +2245,7 @@
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="16"/>
       <c r="C10" s="17"/>
@@ -2049,7 +2278,7 @@
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="11"/>
       <c r="C11" s="13"/>
@@ -2082,7 +2311,7 @@
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="16"/>
       <c r="C12" s="17"/>
@@ -2115,7 +2344,7 @@
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="11"/>
       <c r="C13" s="13"/>
@@ -2148,7 +2377,7 @@
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
     </row>
-    <row r="14" spans="1:31" ht="15" thickBot="1">
+    <row r="14" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
@@ -2181,7 +2410,7 @@
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2214,7 +2443,7 @@
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2247,7 +2476,7 @@
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2280,7 +2509,7 @@
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2313,7 +2542,7 @@
       <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2346,7 +2575,7 @@
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2379,7 +2608,7 @@
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2412,7 +2641,7 @@
       <c r="AD21" s="4"/>
       <c r="AE21" s="4"/>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2445,7 +2674,7 @@
       <c r="AD22" s="4"/>
       <c r="AE22" s="4"/>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2478,7 +2707,7 @@
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2511,7 +2740,7 @@
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2544,7 +2773,7 @@
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2577,7 +2806,7 @@
       <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2610,7 +2839,7 @@
       <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2643,7 +2872,7 @@
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2676,7 +2905,7 @@
       <c r="AD29" s="4"/>
       <c r="AE29" s="4"/>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2709,7 +2938,7 @@
       <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2742,7 +2971,7 @@
       <c r="AD31" s="4"/>
       <c r="AE31" s="4"/>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2775,7 +3004,7 @@
       <c r="AD32" s="4"/>
       <c r="AE32" s="4"/>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2808,7 +3037,7 @@
       <c r="AD33" s="4"/>
       <c r="AE33" s="4"/>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2841,7 +3070,7 @@
       <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2874,7 +3103,7 @@
       <c r="AD35" s="4"/>
       <c r="AE35" s="4"/>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2907,7 +3136,7 @@
       <c r="AD36" s="4"/>
       <c r="AE36" s="4"/>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2940,7 +3169,7 @@
       <c r="AD37" s="4"/>
       <c r="AE37" s="4"/>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2973,7 +3202,7 @@
       <c r="AD38" s="4"/>
       <c r="AE38" s="4"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -3006,7 +3235,7 @@
       <c r="AD39" s="4"/>
       <c r="AE39" s="4"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -3039,7 +3268,7 @@
       <c r="AD40" s="4"/>
       <c r="AE40" s="4"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -3072,7 +3301,7 @@
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3105,7 +3334,7 @@
       <c r="AD42" s="4"/>
       <c r="AE42" s="4"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -3138,7 +3367,7 @@
       <c r="AD43" s="4"/>
       <c r="AE43" s="4"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -3171,7 +3400,7 @@
       <c r="AD44" s="4"/>
       <c r="AE44" s="4"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -3204,7 +3433,7 @@
       <c r="AD45" s="4"/>
       <c r="AE45" s="4"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -3237,7 +3466,7 @@
       <c r="AD46" s="4"/>
       <c r="AE46" s="4"/>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3270,7 +3499,7 @@
       <c r="AD47" s="4"/>
       <c r="AE47" s="4"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -3303,7 +3532,7 @@
       <c r="AD48" s="4"/>
       <c r="AE48" s="4"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -3351,36 +3580,36 @@
   <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P26" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="S49" sqref="S49"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="17.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="30.28515625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="30" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="20.75" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="17.75" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="30.25" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.75" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.75" style="30" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="27.25" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="31" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.25" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8.75" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="6.75" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="79.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
-    <col min="19" max="19" width="92.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.25" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="79.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.25" customWidth="1"/>
+    <col min="18" max="18" width="15.75" customWidth="1"/>
+    <col min="19" max="19" width="92.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="33.6" customHeight="1">
+    <row r="1" spans="1:19" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -3424,7 +3653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18" customHeight="1">
+    <row r="2" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35">
         <v>1</v>
       </c>
@@ -3450,26 +3679,26 @@
         <v>21</v>
       </c>
       <c r="M2" s="37"/>
-      <c r="N2" s="36">
+      <c r="N2" s="81">
         <v>1</v>
       </c>
-      <c r="O2" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="49" t="s">
+      <c r="O2" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="P2" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="49" t="s">
+      <c r="R2" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" s="67" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1">
+      <c r="S2" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40"/>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -3479,437 +3708,439 @@
       <c r="G3" s="43"/>
       <c r="H3" s="41"/>
       <c r="M3" s="37"/>
-      <c r="N3" s="36">
+      <c r="N3" s="81">
         <v>2</v>
       </c>
-      <c r="O3" s="47" t="s">
+      <c r="O3" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="49" t="s">
+      <c r="P3" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="37"/>
+      <c r="N4" s="81">
+        <v>3</v>
+      </c>
+      <c r="O4" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="74" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="37"/>
+      <c r="N5" s="81">
+        <v>4</v>
+      </c>
+      <c r="O5" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q5" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="67" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1">
-      <c r="M4" s="37"/>
-      <c r="N4" s="36">
-        <v>3</v>
-      </c>
-      <c r="O4" s="47" t="s">
+      <c r="R5" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="S5" s="75" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="37"/>
+      <c r="N6" s="81">
+        <v>5</v>
+      </c>
+      <c r="O6" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="49" t="s">
+      <c r="P6" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="67" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1">
-      <c r="M5" s="37"/>
-      <c r="N5" s="36">
-        <v>4</v>
-      </c>
-      <c r="O5" s="47" t="s">
+      <c r="S6" s="74" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="37"/>
+      <c r="N7" s="82">
+        <v>6</v>
+      </c>
+      <c r="O7" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S5" s="45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1">
-      <c r="M6" s="37"/>
-      <c r="N6" s="36">
-        <v>5</v>
-      </c>
-      <c r="O6" s="47" t="s">
+      <c r="P7" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q7" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="74" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="37"/>
+      <c r="N8" s="82">
+        <v>7</v>
+      </c>
+      <c r="O8" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="49" t="s">
+      <c r="P8" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q8" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S6" s="67" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1">
-      <c r="M7" s="37"/>
-      <c r="N7" s="54">
-        <v>6</v>
-      </c>
-      <c r="O7" s="47" t="s">
+      <c r="S8" s="74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="37"/>
+      <c r="N9" s="82">
+        <v>8</v>
+      </c>
+      <c r="O9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="49" t="s">
+      <c r="P9" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q9" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S7" s="67" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="18" customHeight="1">
-      <c r="M8" s="37"/>
-      <c r="N8" s="54">
-        <v>7</v>
-      </c>
-      <c r="O8" s="47" t="s">
+      <c r="S9" s="74" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="37"/>
+      <c r="N10" s="82">
+        <v>9</v>
+      </c>
+      <c r="O10" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q8" s="49" t="s">
+      <c r="P10" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S8" s="67" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1">
-      <c r="M9" s="37"/>
-      <c r="N9" s="54">
-        <v>8</v>
-      </c>
-      <c r="O9" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S9" s="67" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1">
-      <c r="M10" s="37"/>
-      <c r="N10" s="54">
-        <v>9</v>
-      </c>
-      <c r="O10" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q10" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S10" s="67" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1">
+      <c r="S10" s="74" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F11" s="38"/>
       <c r="H11" s="39"/>
-      <c r="N11" s="54">
-        <v>11</v>
-      </c>
-      <c r="O11" s="47" t="s">
+      <c r="N11" s="82">
+        <v>10</v>
+      </c>
+      <c r="O11" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P11" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q11" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S11" s="45" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1">
+      <c r="P11" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q11" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="S11" s="75" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F12" s="38"/>
       <c r="H12" s="39"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="47" t="s">
+      <c r="N12" s="82">
+        <v>11</v>
+      </c>
+      <c r="O12" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q12" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S12" s="45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1">
+      <c r="P12" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q12" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="S12" s="75" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F13" s="38"/>
       <c r="H13" s="39"/>
-      <c r="N13" s="54">
+      <c r="N13" s="82">
         <v>12</v>
       </c>
-      <c r="O13" s="48" t="s">
+      <c r="O13" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="P13" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q13" s="49" t="s">
+      <c r="P13" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q13" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R13" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S13" s="67" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1">
+      <c r="S13" s="74" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F14" s="38"/>
       <c r="H14" s="39"/>
-      <c r="N14" s="54">
+      <c r="N14" s="82">
         <v>13</v>
       </c>
-      <c r="O14" s="63" t="s">
+      <c r="O14" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="P14" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q14" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S14" s="45"/>
-    </row>
-    <row r="15" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1">
+      <c r="P14" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q14" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="R14" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="S14" s="75"/>
+    </row>
+    <row r="15" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F15" s="38"/>
       <c r="H15" s="39"/>
-      <c r="N15" s="54">
+      <c r="N15" s="82">
         <v>14</v>
       </c>
-      <c r="O15" s="64" t="s">
+      <c r="O15" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="P15" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q15" s="49" t="s">
+      <c r="P15" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q15" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R15" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S15" s="67" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1">
+      <c r="S15" s="74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F16" s="38"/>
       <c r="H16" s="39"/>
-      <c r="N16" s="54">
+      <c r="N16" s="82">
         <v>15</v>
       </c>
-      <c r="O16" s="64" t="s">
+      <c r="O16" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q16" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S16" s="45"/>
-    </row>
-    <row r="17" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1">
+      <c r="P16" s="80" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q16" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="R16" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16" s="75"/>
+    </row>
+    <row r="17" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F17" s="38"/>
       <c r="H17" s="39"/>
-      <c r="N17" s="54">
+      <c r="N17" s="82">
         <v>16</v>
       </c>
-      <c r="O17" s="64" t="s">
+      <c r="O17" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="P17" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q17" s="49" t="s">
+      <c r="P17" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q17" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="R17" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S17" s="67" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1">
+      <c r="S17" s="74" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F18" s="38"/>
       <c r="H18" s="39"/>
-      <c r="N18" s="54">
+      <c r="N18" s="52">
         <v>17</v>
       </c>
-      <c r="O18" s="64" t="s">
+      <c r="O18" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="P18" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q18" s="49" t="s">
-        <v>48</v>
+      <c r="P18" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q18" s="47" t="s">
+        <v>28</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S18" s="45"/>
     </row>
-    <row r="19" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1">
+    <row r="19" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F19" s="38"/>
       <c r="H19" s="39"/>
-      <c r="N19" s="54">
+      <c r="N19" s="52">
         <v>18</v>
       </c>
-      <c r="O19" s="65" t="s">
+      <c r="O19" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="P19" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q19" s="49" t="s">
-        <v>61</v>
+      <c r="P19" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q19" s="47" t="s">
+        <v>33</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S19" s="45"/>
     </row>
-    <row r="20" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1">
+    <row r="20" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F20" s="38"/>
       <c r="H20" s="39"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="P20" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q20" s="49"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="P20" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q20" s="47"/>
       <c r="R20" s="3"/>
       <c r="S20" s="45"/>
     </row>
-    <row r="21" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="21" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N21" s="36">
         <v>19</v>
       </c>
-      <c r="O21" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="P21" s="55" t="s">
-        <v>64</v>
+      <c r="O21" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="P21" s="84" t="s">
+        <v>99</v>
       </c>
       <c r="Q21" s="46" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S21" s="45"/>
     </row>
-    <row r="22" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="22" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N22" s="36">
         <v>20</v>
       </c>
-      <c r="O22" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="P22" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q22" s="46" t="s">
-        <v>48</v>
+      <c r="O22" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="P22" s="84" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q22" s="85" t="s">
+        <v>89</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S22" s="45"/>
     </row>
-    <row r="23" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="23" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N23" s="36">
         <v>21</v>
       </c>
-      <c r="O23" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="P23" s="55" t="s">
-        <v>66</v>
+      <c r="O23" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="P23" s="84" t="s">
+        <v>101</v>
       </c>
       <c r="Q23" s="46" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="R23" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S23" s="45"/>
     </row>
-    <row r="24" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="24" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N24" s="36">
         <v>22</v>
       </c>
-      <c r="O24" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P24" s="51" t="s">
-        <v>68</v>
+      <c r="O24" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="P24" s="49" t="s">
+        <v>90</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="3" t="s">
@@ -3917,161 +4148,163 @@
       </c>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="25" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N25" s="36">
         <v>23</v>
       </c>
-      <c r="O25" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P25" s="51" t="s">
-        <v>69</v>
+      <c r="O25" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="P25" s="83" t="s">
+        <v>102</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="R25" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="26" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N26" s="36">
         <v>24</v>
       </c>
-      <c r="O26" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P26" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q26" s="50" t="s">
-        <v>24</v>
+      <c r="O26" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P26" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q26" s="48" t="s">
+        <v>23</v>
       </c>
       <c r="R26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S26" s="67" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="6:19" ht="18" customHeight="1" thickBot="1">
+      <c r="S26" s="62" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N27" s="36">
         <v>25</v>
       </c>
-      <c r="O27" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P27" s="51" t="s">
-        <v>71</v>
+      <c r="O27" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P27" s="83" t="s">
+        <v>104</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="R27" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="28" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N28" s="36">
         <v>26</v>
       </c>
-      <c r="O28" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P28" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>48</v>
+      <c r="O28" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P28" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q28" s="86" t="s">
+        <v>89</v>
       </c>
       <c r="R28" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="29" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N29" s="36">
         <v>27</v>
       </c>
-      <c r="O29" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P29" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>48</v>
+      <c r="O29" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P29" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q29" s="86" t="s">
+        <v>89</v>
       </c>
       <c r="R29" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="30" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N30" s="36">
         <v>28</v>
       </c>
-      <c r="O30" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P30" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>75</v>
+      <c r="O30" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P30" s="83" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q30" s="86" t="s">
+        <v>91</v>
       </c>
       <c r="R30" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="31" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N31" s="36">
         <v>29</v>
       </c>
-      <c r="O31" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P31" s="51" t="s">
-        <v>76</v>
+      <c r="O31" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P31" s="83" t="s">
+        <v>108</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="R31" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="6:19" ht="18" customHeight="1" thickBot="1">
+    <row r="32" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N32" s="36">
         <v>30</v>
       </c>
-      <c r="O32" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P32" s="69" t="s">
-        <v>77</v>
+      <c r="O32" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P32" s="64" t="s">
+        <v>109</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="R32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S32" s="1"/>
-    </row>
-    <row r="33" spans="14:19" ht="18" customHeight="1" thickBot="1">
+      <c r="S32" s="87" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N33" s="36">
         <v>31</v>
       </c>
-      <c r="O33" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P33" s="51" t="s">
-        <v>78</v>
+      <c r="O33" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P33" s="49" t="s">
+        <v>97</v>
       </c>
       <c r="Q33" s="1"/>
       <c r="R33" s="3" t="s">
@@ -4079,340 +4312,342 @@
       </c>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="14:19" ht="18" customHeight="1" thickBot="1">
+    <row r="34" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N34" s="36">
         <v>32</v>
       </c>
-      <c r="O34" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P34" s="51" t="s">
-        <v>79</v>
+      <c r="O34" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P34" s="49" t="s">
+        <v>110</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R34" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S34" s="67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="14:19" ht="18" customHeight="1" thickBot="1">
+      <c r="S34" s="62" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N35" s="36">
         <v>33</v>
       </c>
-      <c r="O35" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P35" s="51" t="s">
-        <v>81</v>
+      <c r="O35" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="P35" s="49" t="s">
+        <v>111</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R35" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S35" s="67" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="14:19" ht="18" customHeight="1" thickBot="1">
+      <c r="S35" s="62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N36" s="36">
         <v>34</v>
       </c>
-      <c r="O36" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P36" s="51" t="s">
-        <v>82</v>
+      <c r="O36" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P36" s="49" t="s">
+        <v>112</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R36" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S36" s="67" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="14:19" ht="18" customHeight="1" thickBot="1">
+      <c r="S36" s="62" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N37" s="36">
         <v>35</v>
       </c>
-      <c r="O37" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="P37" s="69" t="s">
-        <v>84</v>
+      <c r="O37" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P37" s="64" t="s">
+        <v>113</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S37" s="1"/>
-    </row>
-    <row r="38" spans="14:19" ht="18" customHeight="1" thickBot="1">
+      <c r="S37" s="86" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N38" s="36"/>
-      <c r="O38" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P38" s="51" t="s">
-        <v>86</v>
+      <c r="O38" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="P38" s="49" t="s">
+        <v>76</v>
       </c>
       <c r="Q38" s="1"/>
       <c r="R38" s="3"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="14:19" ht="18" customHeight="1" thickBot="1">
+    <row r="39" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N39" s="36">
         <v>36</v>
       </c>
-      <c r="O39" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P39" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q39" s="53" t="s">
-        <v>52</v>
+      <c r="O39" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P39" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q39" s="51" t="s">
+        <v>30</v>
       </c>
       <c r="R39" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="14:19" ht="18" customHeight="1" thickBot="1">
+    <row r="40" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N40" s="36">
         <v>37</v>
       </c>
-      <c r="O40" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P40" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q40" s="53" t="s">
-        <v>52</v>
+      <c r="O40" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P40" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q40" s="51" t="s">
+        <v>30</v>
       </c>
       <c r="R40" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="14:19" ht="18" customHeight="1" thickBot="1">
+    <row r="41" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N41" s="36">
         <v>38</v>
       </c>
-      <c r="O41" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P41" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q41" s="53" t="s">
-        <v>52</v>
+      <c r="O41" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P41" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q41" s="51" t="s">
+        <v>30</v>
       </c>
       <c r="R41" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="14:19" ht="18" customHeight="1" thickBot="1">
+    <row r="42" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N42" s="36">
         <v>39</v>
       </c>
-      <c r="O42" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P42" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q42" s="53" t="s">
-        <v>52</v>
+      <c r="O42" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P42" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q42" s="51" t="s">
+        <v>30</v>
       </c>
       <c r="R42" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="14:19" ht="18" customHeight="1" thickBot="1">
+    <row r="43" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N43" s="36">
         <v>40</v>
       </c>
-      <c r="O43" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P43" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q43" s="53" t="s">
-        <v>52</v>
+      <c r="O43" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P43" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q43" s="51" t="s">
+        <v>30</v>
       </c>
       <c r="R43" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="14:19" ht="18" customHeight="1" thickBot="1">
+    <row r="44" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N44" s="36">
         <v>41</v>
       </c>
-      <c r="O44" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P44" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q44" s="52" t="s">
-        <v>56</v>
+      <c r="O44" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P44" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q44" s="50" t="s">
+        <v>32</v>
       </c>
       <c r="R44" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="14:19" ht="18" customHeight="1" thickBot="1">
+    <row r="45" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N45" s="36">
         <v>42</v>
       </c>
-      <c r="O45" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P45" s="51" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q45" s="52" t="s">
-        <v>94</v>
+      <c r="O45" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P45" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q45" s="50" t="s">
+        <v>40</v>
       </c>
       <c r="R45" s="3" t="s">
         <v>20</v>
       </c>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="14:19" ht="34.9" customHeight="1" thickBot="1">
+    <row r="46" spans="14:19" ht="34.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N46" s="36">
         <v>43</v>
       </c>
-      <c r="O46" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P46" s="51" t="s">
-        <v>95</v>
+      <c r="O46" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P46" s="49" t="s">
+        <v>121</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R46" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S46" s="68" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="14:19" ht="18" customHeight="1" thickBot="1">
+      <c r="S46" s="63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N47" s="36">
         <v>44</v>
       </c>
-      <c r="O47" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P47" s="51" t="s">
-        <v>97</v>
+      <c r="O47" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P47" s="49" t="s">
+        <v>122</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R47" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S47" s="68" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="14:19" ht="18" customHeight="1" thickBot="1">
+      <c r="S47" s="63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N48" s="36">
         <v>45</v>
       </c>
-      <c r="O48" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="P48" s="51" t="s">
-        <v>99</v>
+      <c r="O48" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="P48" s="49" t="s">
+        <v>123</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R48" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S48" s="68" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="14:19" ht="18" customHeight="1">
+      <c r="S48" s="63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="14:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N49" s="36">
         <v>46</v>
       </c>
-      <c r="O49" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="P49" s="60" t="s">
-        <v>101</v>
+      <c r="O49" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="P49" s="57" t="s">
+        <v>85</v>
       </c>
       <c r="Q49" s="46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R49" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S49" s="67" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="14:19" ht="18" customHeight="1">
+      <c r="S49" s="62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="14:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N50" s="36">
         <v>47</v>
       </c>
-      <c r="O50" s="57" t="s">
-        <v>100</v>
-      </c>
-      <c r="P50" s="61" t="s">
-        <v>103</v>
+      <c r="O50" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="P50" s="58" t="s">
+        <v>86</v>
       </c>
       <c r="Q50" s="46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R50" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S50" s="67" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="14:19" ht="18" customHeight="1" thickBot="1">
+      <c r="S50" s="62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N51" s="36">
         <v>48</v>
       </c>
-      <c r="O51" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="P51" s="61" t="s">
-        <v>105</v>
+      <c r="O51" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="P51" s="58" t="s">
+        <v>88</v>
       </c>
       <c r="Q51" s="46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R51" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S51" s="67" t="s">
-        <v>41</v>
+      <c r="S51" s="62" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -4468,122 +4703,122 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.125" customWidth="1"/>
+    <col min="2" max="2" width="49.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.25" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A1" s="73" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="74" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
+    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
       <c r="C2" s="24" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="F2" s="25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="E4" s="36"/>
       <c r="F4" s="36"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
     </row>
-    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1">
+    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="44" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="36" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="F6" s="36"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
-        <v>114</v>
+        <v>52</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36"/>
       <c r="F7" s="36" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -4627,16 +4862,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x01010092279BF5F3BBB64297C5CD812DA5D812" ma:contentTypeVersion="11" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="b68580309290129f5a0b6aa152431cc7">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b0add36e-da03-4abd-a3e0-9f2a80588293" xmlns:ns3="ce510894-e256-4a70-bf8c-71462871c739" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="72820fed29527527b21b83f152d5137a" ns2:_="" ns3:_="">
-    <xsd:import namespace="b0add36e-da03-4abd-a3e0-9f2a80588293"/>
-    <xsd:import namespace="ce510894-e256-4a70-bf8c-71462871c739"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033C8C618B2A2B341B3B0C9790A173ACD" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d8daa8148d049b84ea5d859d5c43d1f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9" xmlns:ns3="a0b74ea9-89d9-43cb-a163-e9320d483776" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c59df6f59bfc848cd60a2150922ac339" ns2:_="" ns3:_="">
+    <xsd:import namespace="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9"/>
+    <xsd:import namespace="a0b74ea9-89d9-43cb-a163-e9320d483776"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -4645,15 +4874,13 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4661,7 +4888,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b0add36e-da03-4abd-a3e0-9f2a80588293" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -4674,39 +4901,27 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="17" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="18" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceKeyPoints" ma:index="14" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -4714,10 +4929,10 @@
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ce510894-e256-4a70-bf8c-71462871c739" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a0b74ea9-89d9-43cb-a163-e9320d483776" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="공유 대상" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -4736,7 +4951,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="세부 정보 공유" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -4753,8 +4968,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="콘텐츠 형식"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="제목"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -4843,6 +5058,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4853,13 +5074,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEA00D43-58AE-47FC-B235-F2B32D6A0948}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F66E58E-3B26-4919-8626-35E46A28D673}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
upload 4 signal matrixs for R2 SW release from IBT
</commit_message>
<xml_diff>
--- a/R2/02_SignalMatrix/HkmcFcaAdap/HkmcFcaAdap_SignalMatrix_V1.xlsx
+++ b/R2/02_SignalMatrix/HkmcFcaAdap/HkmcFcaAdap_SignalMatrix_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soo-jin.ahn\Veoneer\KHT HKMC BN7 FCA Project - SOS and MVS4\01_Engineering\03_SW and FD\ApplicationSoftware\FeatureSignalMatrixs\HkmcFcaAdap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{345847E7-D56C-41D3-9BD6-A37BFB0E82E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B10CF31-E1AB-48F8-ABB8-75381FF14C64}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="13_ncr:1_{345847E7-D56C-41D3-9BD6-A37BFB0E82E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{191440B1-A19A-42F9-89E3-AAE5359B7C56}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="22" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="131">
   <si>
     <t>Change Log</t>
   </si>
@@ -157,9 +157,6 @@
     <t>uint8</t>
   </si>
   <si>
-    <t>[0..2.55] ,0.01</t>
-  </si>
-  <si>
     <t>u16</t>
   </si>
   <si>
@@ -172,15 +169,6 @@
     <t>S16</t>
   </si>
   <si>
-    <t>Cx0_Unknown
-Cx1_Car
-Cx2_Motorcycle
-Cx3_Truck
-Cx4_Pedestrian
-Cx5_Bicycle
-Cx6_GeneralObject</t>
-  </si>
-  <si>
     <t>boolean</t>
   </si>
   <si>
@@ -196,14 +184,6 @@
     <t>ASP_CollisionMitigationSystem</t>
   </si>
   <si>
-    <t>Cx0_NoMessage
-Cx1_InterventionLongitudinal
-Cx2_InterventionLateral
-Cx3_InterventionLongitudinalAndInterventionLateral
-Cx4_BrakePulse
-Cx5_CriteriaBrakeMessage</t>
-  </si>
-  <si>
     <t>ASP_EgoMotionOutput</t>
   </si>
   <si>
@@ -213,16 +193,6 @@
     <t>U32</t>
   </si>
   <si>
-    <t>Cx0_Unknown_x000D_
-Cx1_SuccessfulVerification_x000D_
-Cx2_VerificationFailed</t>
-  </si>
-  <si>
-    <t>Cx0_Unknown
-Cx1_SuccessfulVerification
-Cx2_VerificationFailed</t>
-  </si>
-  <si>
     <t>HVIA_CLU</t>
   </si>
   <si>
@@ -253,13 +223,6 @@
   </si>
   <si>
     <t>HkmcVehicleOutPutAdap</t>
-  </si>
-  <si>
-    <t>Cx0_kmperh
-Cx1_MPH
-Cx2_Not_used
-Cx3_Error_Indicator</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_NoActivation
@@ -273,67 +236,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Cx0_No_warning
-Cx1_Warning_Level_1
-Cx2_Warning_Level_2
-Cx3_Warning_Level_3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_No_Pre_fill
-Cx1_Pre_fill_act
-Cx2_Reserved
-Cx3_Error_Indicator</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_No_Full_act
-Cx1_Full_act
-Cx2_Reserved
-Cx3_Error_Indicator</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_Release_no_alert
-Cx1_Precrash_full_retraction
-Cx2_Haptic_Warning
-Cx3_Reserved
-Cx4_Reserved
-Cx5_Reserved
-Cx6_Reserved
-Cx7_Reserved</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_No_Request
-Cx1_Stop_control_is_required
-Cx2_Reserved
-Cx3_Error_Indicator</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_Default
-Cx1_Off
-Cx2_Warning
-Cx3_Assist
-Cx4_Reserved
-Cx5_Reserved
-Cx6_Reserved
-Cx7_Invalid</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_Normal
-Cx1_Temp_Unavailable_by_Camera
-Cx2_Temp_Unavailable_by_Radar
-Cx3_Service_Required
-Cx4_Temp_Unavailable_by_Camera
-Cx5_Reserved
-Cx6_Reserved
-Cx7_Reserved</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>FcaAdap_SnstvtyModRetVal</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -342,27 +244,10 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Cx0_Unknown
-Cx1_Car
-Cx2_Motorcycle
-Cx3_Truck
-Cx4_Pedestrian
-Cx5_Bicycle
-Cx6_GeneralObject</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>FcaAdap_CollisionThreatLevel</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Cx0_Unknown
-Cx1_ThreatLow
-Cx2_ThreatMedium
-Cx3_ThreatHigh</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>FcaAdap_WrngLvlSta</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -436,17 +321,6 @@
   </si>
   <si>
     <t>HkmcVehicleInput_Fca1stWrngSetReq</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_Default
-Cx1_LDW_Mode
-Cx2_LKA_Mode
-Cx3_Reserved
-Cx4_Reserved
-Cx5_Reserved
-Cx6_Reserved
-Cx7_Invalid</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -660,6 +534,183 @@
   </si>
   <si>
     <t>HFA_OUTPUTS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_WrngLS_No_warning
+Cx1_WrngLS_Warning_Level_1
+Cx2_WrngLS_Warning_Level_2
+Cx3_WrngLS_Warning_Level_3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_WrngSS_No_warning
+Cx1_WrngSS_Warning_Level_1
+Cx2_WrngSS_Warning_Level_2
+Cx3_WrngSS_Warning_Level_3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0..2.55] ,0.01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_PrefillAR_No_Pre_fill
+Cx1_PrefillAR_Pre_fill_act
+Cx2_PrefillAR_Reserved
+Cx3_PrefillAR_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_FullAR_No_Full_act
+Cx1_FullAR_Full_act
+Cx2_FullAR_Reserved
+Cx3_FullAR_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_OnOffES_Default
+Cx1_OnOffES_Off
+Cx2_OnOffES_Warning
+Cx3_OnOffES_Assist
+Cx4_OnOffES_Reserved
+Cx5_OnOffES_Reserved
+Cx6_OnOffES_Reserved
+Cx7_OnOffES_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_NoMessage
+Cx1_InterventionLongitudinal
+Cx2_InterventionLateral
+Cx3_InterventionLongitudinalAndInterventionLateral
+Cx4_BrakePulse
+Cx5_CriteriaBrakeMessage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_SysFlrS_Normal
+Cx1_SysFlrS_Temp_Unavailable_by_Camera
+Cx2_SysFlrS_Temp_Unavailable_by_Radar
+Cx3_SysFlrS_Service_Required
+Cx4_SysFlrS_Temp_Unavailable_by_Camera
+Cx5_SysFlrS_Reserved
+Cx6_SysFlrS_Reserved
+Cx7_SysFlrS_Reserved</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_LongV_Default
+Cx1_LongV_Off
+Cx2_LongV_Warning
+Cx3_LongV_Assist
+Cx4_LongV_Reserved
+Cx5_LongV_Reserved
+Cx6_LongV_Reserved
+Cx7_LongV_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_CollisionTL_Unknown
+Cx1_CollisionTL_ThreatLow
+Cx2_CollisionTL_ThreatMedium
+Cx3_CollisionTL_ThreatHigh</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_ObT_Unknown
+Cx1_ObT_Car
+Cx2_ObT_Motorcycle
+Cx3_ObT_Truck
+Cx4_ObT_Pedestrian
+Cx5_ObT_Bicycle
+Cx6_ObT_GeneralObject</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_ASPObT_Unknown
+Cx1_ASPObT_Car
+Cx2_ASPObT_Motorcycle
+Cx3_ASPObT_Truck
+Cx4_ASPObT_Pedestrian
+Cx5_ASPObT_Bicycle
+Cx6_ASPObT_GeneralObject</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_ASPCollisionTL_Unknown
+Cx1_ASPCollisionTL_ThreatLow
+Cx2_ASPCollisionTL_ThreatMedium
+Cx3_ASPCollisionTL_ThreatHigh</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_LongVS_Unknown
+Cx1_LongVS_SuccessfulVerification
+Cx2_LongVS_VerificationFailed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AccelerationS_Unknown
+Cx1_AccelerationS_SuccessfulVerification
+Cx2_AccelerationS_VerificationFailed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_YawRateS_Unknown
+Cx1_YawRateS_SuccessfulVerification
+Cx2_YawRateS_VerificationFailed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_SpdUT_kmperh
+Cx1_SpdUT_MPH
+Cx2_SpdUT_Not_used
+Cx3_SpdUT_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_Fca1stWSR_Default
+Cx1_Fca1stWSR_LDW_Mode
+Cx2_Fca1stWSR_LKA_Mode
+Cx3_Fca1stWSR_Reserved
+Cx4_Fca1stWSR_Reserved
+Cx5_Fca1stWSR_Reserved
+Cx6_Fca1stWSR_Reserved
+Cx7_Fca1stWSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasFCASR_Default
+Cx1_AdasFCASR_Off
+Cx2_AdasFCASR_Warning
+Cx3_AdasFCASR_Assist
+Cx4_AdasFCASR_Reserved
+Cx5_AdasFCASR_Reserved
+Cx6_AdasFCASR_Reserved
+Cx7_AdasFCASR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_VehSR_No_Request
+Cx1_VehSR_Stop_control_is_required
+Cx2_VehSR_Reserved
+Cx3_VehSR_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_StbltAR_Release_no_alert
+Cx1_StbltAR_Precrash_full_retraction
+Cx2_StbltAR_Haptic_Warning
+Cx3_StbltAR_Reserved
+Cx4_StbltAR_Reserved
+Cx5_StbltAR_Reserved
+Cx6_StbltAR_Reserved
+Cx7_StbltAR_Reserved</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HVIA_CLU</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1412,24 +1463,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1468,6 +1501,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Good" xfId="13" builtinId="26"/>
@@ -1996,13 +2047,13 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="67"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -3580,10 +3631,10 @@
   <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T21" sqref="T21"/>
+      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -3603,7 +3654,7 @@
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="5.875" style="33" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="40.25" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="79.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="75.125" customWidth="1"/>
     <col min="17" max="17" width="14.25" customWidth="1"/>
     <col min="18" max="18" width="15.75" customWidth="1"/>
     <col min="19" max="19" width="92.25" bestFit="1" customWidth="1"/>
@@ -3679,23 +3730,23 @@
         <v>21</v>
       </c>
       <c r="M2" s="37"/>
-      <c r="N2" s="81">
+      <c r="N2" s="75">
         <v>1</v>
       </c>
-      <c r="O2" s="71" t="s">
-        <v>124</v>
-      </c>
-      <c r="P2" s="72" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q2" s="72" t="s">
+      <c r="O2" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="73" t="s">
+      <c r="R2" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="74" t="s">
-        <v>56</v>
+      <c r="S2" s="68" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -3708,320 +3759,320 @@
       <c r="G3" s="43"/>
       <c r="H3" s="41"/>
       <c r="M3" s="37"/>
-      <c r="N3" s="81">
+      <c r="N3" s="75">
         <v>2</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q3" s="72" t="s">
+      <c r="P3" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="73" t="s">
+      <c r="R3" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="74" t="s">
-        <v>56</v>
+      <c r="S3" s="68" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M4" s="37"/>
-      <c r="N4" s="81">
+      <c r="N4" s="75">
         <v>3</v>
       </c>
-      <c r="O4" s="71" t="s">
+      <c r="O4" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="72" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q4" s="72" t="s">
+      <c r="P4" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="73" t="s">
+      <c r="R4" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S4" s="74" t="s">
-        <v>57</v>
+      <c r="S4" s="68" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M5" s="37"/>
-      <c r="N5" s="81">
+      <c r="N5" s="75">
         <v>4</v>
       </c>
-      <c r="O5" s="71" t="s">
+      <c r="O5" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q5" s="72" t="s">
+      <c r="P5" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="R5" s="73" t="s">
+      <c r="R5" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S5" s="75" t="s">
-        <v>26</v>
+      <c r="S5" s="69" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M6" s="37"/>
-      <c r="N6" s="81">
+      <c r="N6" s="75">
         <v>5</v>
       </c>
-      <c r="O6" s="71" t="s">
+      <c r="O6" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q6" s="72" t="s">
+      <c r="P6" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R6" s="73" t="s">
+      <c r="R6" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S6" s="74" t="s">
-        <v>58</v>
+      <c r="S6" s="68" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M7" s="37"/>
-      <c r="N7" s="82">
+      <c r="N7" s="76">
         <v>6</v>
       </c>
-      <c r="O7" s="71" t="s">
+      <c r="O7" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q7" s="72" t="s">
+      <c r="P7" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R7" s="73" t="s">
+      <c r="R7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S7" s="74" t="s">
-        <v>59</v>
+      <c r="S7" s="68" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M8" s="37"/>
-      <c r="N8" s="82">
+      <c r="N8" s="76">
         <v>7</v>
       </c>
-      <c r="O8" s="71" t="s">
+      <c r="O8" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="72" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q8" s="72" t="s">
+      <c r="P8" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="73" t="s">
+      <c r="R8" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S8" s="74" t="s">
-        <v>60</v>
+      <c r="S8" s="68" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M9" s="37"/>
-      <c r="N9" s="82">
+      <c r="N9" s="76">
         <v>8</v>
       </c>
-      <c r="O9" s="71" t="s">
+      <c r="O9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P9" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q9" s="72" t="s">
+      <c r="P9" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q9" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R9" s="73" t="s">
+      <c r="R9" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S9" s="74" t="s">
-        <v>61</v>
+      <c r="S9" s="68" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M10" s="37"/>
-      <c r="N10" s="82">
+      <c r="N10" s="76">
         <v>9</v>
       </c>
-      <c r="O10" s="71" t="s">
+      <c r="O10" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q10" s="72" t="s">
+      <c r="P10" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q10" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="73" t="s">
+      <c r="R10" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S10" s="74" t="s">
-        <v>62</v>
+      <c r="S10" s="68" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F11" s="38"/>
       <c r="H11" s="39"/>
-      <c r="N11" s="82">
+      <c r="N11" s="76">
         <v>10</v>
       </c>
-      <c r="O11" s="71" t="s">
+      <c r="O11" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P11" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q11" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="R11" s="73" t="s">
+      <c r="P11" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q11" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="R11" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S11" s="75" t="s">
-        <v>55</v>
+      <c r="S11" s="69" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F12" s="38"/>
       <c r="H12" s="39"/>
-      <c r="N12" s="82">
+      <c r="N12" s="76">
         <v>11</v>
       </c>
-      <c r="O12" s="71" t="s">
+      <c r="O12" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="72" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q12" s="72" t="s">
+      <c r="P12" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q12" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="R12" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="S12" s="69" t="s">
         <v>28</v>
-      </c>
-      <c r="R12" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="S12" s="75" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F13" s="38"/>
       <c r="H13" s="39"/>
-      <c r="N13" s="82">
+      <c r="N13" s="76">
         <v>12</v>
       </c>
-      <c r="O13" s="76" t="s">
+      <c r="O13" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="P13" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q13" s="72" t="s">
+      <c r="P13" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R13" s="73" t="s">
+      <c r="R13" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S13" s="74" t="s">
-        <v>61</v>
+      <c r="S13" s="68" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F14" s="38"/>
       <c r="H14" s="39"/>
-      <c r="N14" s="82">
+      <c r="N14" s="76">
         <v>13</v>
       </c>
-      <c r="O14" s="77" t="s">
+      <c r="O14" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P14" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q14" s="72" t="s">
-        <v>30</v>
-      </c>
-      <c r="R14" s="73" t="s">
+      <c r="P14" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q14" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S14" s="75"/>
+      <c r="S14" s="69"/>
     </row>
     <row r="15" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F15" s="38"/>
       <c r="H15" s="39"/>
-      <c r="N15" s="82">
+      <c r="N15" s="76">
         <v>14</v>
       </c>
-      <c r="O15" s="79" t="s">
+      <c r="O15" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="P15" s="80" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q15" s="72" t="s">
+      <c r="P15" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q15" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R15" s="73" t="s">
+      <c r="R15" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S15" s="74" t="s">
-        <v>65</v>
+      <c r="S15" s="68" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F16" s="38"/>
       <c r="H16" s="39"/>
-      <c r="N16" s="82">
+      <c r="N16" s="76">
         <v>15</v>
       </c>
-      <c r="O16" s="79" t="s">
+      <c r="O16" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q16" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="R16" s="73" t="s">
+      <c r="P16" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q16" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="R16" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S16" s="75"/>
+      <c r="S16" s="69"/>
     </row>
     <row r="17" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F17" s="38"/>
       <c r="H17" s="39"/>
-      <c r="N17" s="82">
+      <c r="N17" s="76">
         <v>16</v>
       </c>
-      <c r="O17" s="79" t="s">
+      <c r="O17" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="P17" s="80" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q17" s="72" t="s">
+      <c r="P17" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="R17" s="73" t="s">
+      <c r="R17" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="S17" s="74" t="s">
-        <v>67</v>
+      <c r="S17" s="68" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="6:19" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4034,10 +4085,10 @@
         <v>22</v>
       </c>
       <c r="P18" s="59" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="Q18" s="47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>24</v>
@@ -4054,10 +4105,10 @@
         <v>22</v>
       </c>
       <c r="P19" s="59" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="Q19" s="47" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R19" s="3" t="s">
         <v>24</v>
@@ -4069,10 +4120,10 @@
       <c r="H20" s="39"/>
       <c r="N20" s="52"/>
       <c r="O20" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="P20" s="88" t="s">
-        <v>95</v>
+        <v>79</v>
+      </c>
+      <c r="P20" s="82" t="s">
+        <v>79</v>
       </c>
       <c r="Q20" s="47"/>
       <c r="R20" s="3"/>
@@ -4083,13 +4134,13 @@
         <v>19</v>
       </c>
       <c r="O21" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="P21" s="84" t="s">
-        <v>99</v>
+        <v>32</v>
+      </c>
+      <c r="P21" s="78" t="s">
+        <v>83</v>
       </c>
       <c r="Q21" s="46" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>20</v>
@@ -4101,13 +4152,13 @@
         <v>20</v>
       </c>
       <c r="O22" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="P22" s="84" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q22" s="85" t="s">
-        <v>89</v>
+        <v>32</v>
+      </c>
+      <c r="P22" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q22" s="79" t="s">
+        <v>73</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>20</v>
@@ -4119,13 +4170,13 @@
         <v>21</v>
       </c>
       <c r="O23" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="P23" s="84" t="s">
-        <v>101</v>
+        <v>32</v>
+      </c>
+      <c r="P23" s="78" t="s">
+        <v>85</v>
       </c>
       <c r="Q23" s="46" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R23" s="3" t="s">
         <v>20</v>
@@ -4137,10 +4188,10 @@
         <v>22</v>
       </c>
       <c r="O24" s="53" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="P24" s="49" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="3" t="s">
@@ -4153,13 +4204,13 @@
         <v>23</v>
       </c>
       <c r="O25" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="P25" s="83" t="s">
-        <v>102</v>
+        <v>80</v>
+      </c>
+      <c r="P25" s="77" t="s">
+        <v>86</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R25" s="3" t="s">
         <v>20</v>
@@ -4171,10 +4222,10 @@
         <v>24</v>
       </c>
       <c r="O26" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="P26" s="83" t="s">
-        <v>103</v>
+        <v>34</v>
+      </c>
+      <c r="P26" s="77" t="s">
+        <v>87</v>
       </c>
       <c r="Q26" s="48" t="s">
         <v>23</v>
@@ -4183,7 +4234,7 @@
         <v>20</v>
       </c>
       <c r="S26" s="62" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="6:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4191,13 +4242,13 @@
         <v>25</v>
       </c>
       <c r="O27" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="P27" s="83" t="s">
-        <v>104</v>
+        <v>34</v>
+      </c>
+      <c r="P27" s="77" t="s">
+        <v>88</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R27" s="3" t="s">
         <v>20</v>
@@ -4209,13 +4260,13 @@
         <v>26</v>
       </c>
       <c r="O28" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="P28" s="83" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q28" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="P28" s="77" t="s">
         <v>89</v>
+      </c>
+      <c r="Q28" s="80" t="s">
+        <v>73</v>
       </c>
       <c r="R28" s="3" t="s">
         <v>20</v>
@@ -4227,13 +4278,13 @@
         <v>27</v>
       </c>
       <c r="O29" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="P29" s="83" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q29" s="86" t="s">
-        <v>89</v>
+        <v>34</v>
+      </c>
+      <c r="P29" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q29" s="80" t="s">
+        <v>73</v>
       </c>
       <c r="R29" s="3" t="s">
         <v>20</v>
@@ -4245,13 +4296,13 @@
         <v>28</v>
       </c>
       <c r="O30" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="P30" s="83" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q30" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="P30" s="77" t="s">
         <v>91</v>
+      </c>
+      <c r="Q30" s="80" t="s">
+        <v>75</v>
       </c>
       <c r="R30" s="3" t="s">
         <v>20</v>
@@ -4263,13 +4314,13 @@
         <v>29</v>
       </c>
       <c r="O31" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="P31" s="83" t="s">
-        <v>108</v>
+        <v>34</v>
+      </c>
+      <c r="P31" s="77" t="s">
+        <v>92</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R31" s="3" t="s">
         <v>20</v>
@@ -4281,19 +4332,19 @@
         <v>30</v>
       </c>
       <c r="O32" s="53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P32" s="64" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="R32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S32" s="87" t="s">
-        <v>92</v>
+      <c r="S32" s="81" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4301,10 +4352,10 @@
         <v>31</v>
       </c>
       <c r="O33" s="53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P33" s="49" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="Q33" s="1"/>
       <c r="R33" s="3" t="s">
@@ -4317,10 +4368,10 @@
         <v>32</v>
       </c>
       <c r="O34" s="53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P34" s="49" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>23</v>
@@ -4329,7 +4380,7 @@
         <v>20</v>
       </c>
       <c r="S34" s="62" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4337,10 +4388,10 @@
         <v>33</v>
       </c>
       <c r="O35" s="53" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="P35" s="49" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>23</v>
@@ -4349,7 +4400,7 @@
         <v>20</v>
       </c>
       <c r="S35" s="62" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4357,10 +4408,10 @@
         <v>34</v>
       </c>
       <c r="O36" s="53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P36" s="49" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>23</v>
@@ -4369,7 +4420,7 @@
         <v>20</v>
       </c>
       <c r="S36" s="62" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4377,10 +4428,10 @@
         <v>35</v>
       </c>
       <c r="O37" s="53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P37" s="64" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>23</v>
@@ -4388,17 +4439,17 @@
       <c r="R37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S37" s="86" t="s">
-        <v>94</v>
+      <c r="S37" s="80" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N38" s="36"/>
       <c r="O38" s="53" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="P38" s="49" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="Q38" s="1"/>
       <c r="R38" s="3"/>
@@ -4409,13 +4460,13 @@
         <v>36</v>
       </c>
       <c r="O39" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P39" s="56" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="Q39" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R39" s="3" t="s">
         <v>20</v>
@@ -4427,13 +4478,13 @@
         <v>37</v>
       </c>
       <c r="O40" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P40" s="49" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="Q40" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R40" s="3" t="s">
         <v>20</v>
@@ -4445,13 +4496,13 @@
         <v>38</v>
       </c>
       <c r="O41" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P41" s="49" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="Q41" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R41" s="3" t="s">
         <v>20</v>
@@ -4463,13 +4514,13 @@
         <v>39</v>
       </c>
       <c r="O42" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P42" s="49" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="Q42" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R42" s="3" t="s">
         <v>20</v>
@@ -4481,13 +4532,13 @@
         <v>40</v>
       </c>
       <c r="O43" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P43" s="49" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="Q43" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R43" s="3" t="s">
         <v>20</v>
@@ -4499,13 +4550,13 @@
         <v>41</v>
       </c>
       <c r="O44" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P44" s="49" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="Q44" s="50" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R44" s="3" t="s">
         <v>20</v>
@@ -4517,13 +4568,13 @@
         <v>42</v>
       </c>
       <c r="O45" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P45" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q45" s="50" t="s">
-        <v>40</v>
+        <v>104</v>
+      </c>
+      <c r="Q45" s="51" t="s">
+        <v>37</v>
       </c>
       <c r="R45" s="3" t="s">
         <v>20</v>
@@ -4535,10 +4586,10 @@
         <v>43</v>
       </c>
       <c r="O46" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P46" s="49" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="Q46" s="1" t="s">
         <v>23</v>
@@ -4547,7 +4598,7 @@
         <v>20</v>
       </c>
       <c r="S46" s="63" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4555,10 +4606,10 @@
         <v>44</v>
       </c>
       <c r="O47" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P47" s="49" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="Q47" s="1" t="s">
         <v>23</v>
@@ -4567,7 +4618,7 @@
         <v>20</v>
       </c>
       <c r="S47" s="63" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4575,10 +4626,10 @@
         <v>45</v>
       </c>
       <c r="O48" s="53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P48" s="49" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="Q48" s="1" t="s">
         <v>23</v>
@@ -4587,7 +4638,7 @@
         <v>20</v>
       </c>
       <c r="S48" s="63" t="s">
-        <v>42</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="14:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4595,10 +4646,10 @@
         <v>46</v>
       </c>
       <c r="O49" s="53" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="P49" s="57" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="Q49" s="46" t="s">
         <v>23</v>
@@ -4607,7 +4658,7 @@
         <v>20</v>
       </c>
       <c r="S49" s="62" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="14:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4615,10 +4666,10 @@
         <v>47</v>
       </c>
       <c r="O50" s="54" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="P50" s="58" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="Q50" s="46" t="s">
         <v>23</v>
@@ -4627,7 +4678,7 @@
         <v>20</v>
       </c>
       <c r="S50" s="62" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="14:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4635,10 +4686,10 @@
         <v>48</v>
       </c>
       <c r="O51" s="55" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="P51" s="58" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="Q51" s="46" t="s">
         <v>23</v>
@@ -4647,7 +4698,7 @@
         <v>20</v>
       </c>
       <c r="S51" s="62" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -4714,28 +4765,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="A1" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="86"/>
+      <c r="C1" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="68"/>
-      <c r="B2" s="68"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="86"/>
       <c r="C2" s="24" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F2" s="25" t="s">
         <v>22</v>
@@ -4743,71 +4794,71 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E4" s="36"/>
       <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="44" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F6" s="36"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>22</v>
@@ -4818,7 +4869,7 @@
       <c r="D7" s="36"/>
       <c r="E7" s="36"/>
       <c r="F7" s="36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -4862,8 +4913,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033C8C618B2A2B341B3B0C9790A173ACD" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d8daa8148d049b84ea5d859d5c43d1f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9" xmlns:ns3="a0b74ea9-89d9-43cb-a163-e9320d483776" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c59df6f59bfc848cd60a2150922ac339" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033C8C618B2A2B341B3B0C9790A173ACD" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c40ebbfe3c414d1ccb793c7a71656a68">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9" xmlns:ns3="a0b74ea9-89d9-43cb-a163-e9320d483776" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f1d82c05e8c45e199eba9dcfb260b401" ns2:_="" ns3:_="">
     <xsd:import namespace="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9"/>
     <xsd:import namespace="a0b74ea9-89d9-43cb-a163-e9320d483776"/>
     <xsd:element name="properties">
@@ -4881,6 +4947,7 @@
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4922,6 +4989,13 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceKeyPoints" ma:index="14" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -5058,38 +5132,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEA00D43-58AE-47FC-B235-F2B32D6A0948}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="a0b74ea9-89d9-43cb-a163-e9320d483776"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93BAE251-9F51-479D-A845-32630E444A76}"/>
 </file>
</xml_diff>